<commit_message>
Gantt Final excel + pdf
</commit_message>
<xml_diff>
--- a/resources/DocumentoPresentacion/Gantt/Gantt project planner1.xlsx
+++ b/resources/DocumentoPresentacion/Gantt/Gantt project planner1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="19200" windowHeight="6540" tabRatio="352"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -29,15 +29,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Plan</t>
   </si>
   <si>
     <t>Actual</t>
-  </si>
-  <si>
-    <t>ACTUAL</t>
   </si>
   <si>
     <r>
@@ -216,12 +213,24 @@
   <si>
     <t>Pruebas</t>
   </si>
+  <si>
+    <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>Documento Versión 2.0</t>
+  </si>
+  <si>
+    <t>Codificación Paquete Controlador</t>
+  </si>
+  <si>
+    <t>Documento Versión 3.0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -350,8 +359,16 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.5"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,8 +434,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -470,6 +493,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -495,7 +527,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -581,6 +613,30 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,9 +656,6 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -616,16 +669,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <fill>
         <patternFill>
@@ -742,6 +786,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -753,17 +825,452 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
         </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
           <color theme="7"/>
-        </top>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -904,7 +1411,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="17"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="52"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1189,20 +1696,20 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:CU34"/>
+  <dimension ref="B2:CU27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="30.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="0.25" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="0.125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="15.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.25" style="1" customWidth="1"/>
     <col min="9" max="9" width="3.5" style="1" customWidth="1"/>
@@ -1233,39 +1740,39 @@
     <col min="79" max="79" width="3.375" bestFit="1" customWidth="1"/>
     <col min="80" max="88" width="3.75" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="90" max="93" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="90" max="99" width="3.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:99" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33" t="s">
+      <c r="B2" s="40" t="s">
         <v>27</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:99" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
       <c r="N3" s="9">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1278,11 +1785,11 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -1290,17 +1797,17 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="28"/>
       <c r="AL3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
@@ -1313,7 +1820,7 @@
       <c r="CB4" s="1"/>
     </row>
     <row r="5" spans="2:99" x14ac:dyDescent="0.3">
-      <c r="H5" s="33"/>
+      <c r="H5" s="41"/>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
@@ -1321,113 +1828,136 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="2:99" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:99" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
-      <c r="AE6" s="35"/>
-      <c r="AF6" s="35"/>
-      <c r="AG6" s="35"/>
-      <c r="AH6" s="35"/>
-      <c r="AI6" s="35"/>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="35"/>
-      <c r="AL6" s="35"/>
-      <c r="AM6" s="30" t="s">
+      <c r="H6" s="41"/>
+      <c r="I6" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AN6" s="30"/>
-      <c r="AO6" s="30"/>
-      <c r="AP6" s="30"/>
-      <c r="AQ6" s="30"/>
-      <c r="AR6" s="30"/>
-      <c r="AS6" s="30"/>
-      <c r="AT6" s="30"/>
-      <c r="AU6" s="30"/>
-      <c r="AV6" s="30"/>
-      <c r="AW6" s="30"/>
-      <c r="AX6" s="30"/>
-      <c r="AY6" s="30"/>
-      <c r="AZ6" s="30"/>
-      <c r="BA6" s="30"/>
-      <c r="BB6" s="30"/>
-      <c r="BC6" s="30"/>
-      <c r="BD6" s="30"/>
-      <c r="BE6" s="30"/>
-      <c r="BF6" s="30"/>
-      <c r="BG6" s="30"/>
-      <c r="BH6" s="30"/>
-      <c r="BI6" s="30"/>
-      <c r="BJ6" s="30"/>
-      <c r="BK6" s="30"/>
-      <c r="BL6" s="30"/>
-      <c r="BM6" s="30"/>
-      <c r="BN6" s="30"/>
-      <c r="BO6" s="30"/>
-      <c r="BP6" s="30"/>
-      <c r="BQ6" s="30"/>
-      <c r="BX6" s="1"/>
-      <c r="BY6" s="1"/>
-      <c r="BZ6" s="1"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="43"/>
+      <c r="X6" s="43"/>
+      <c r="Y6" s="43"/>
+      <c r="Z6" s="43"/>
+      <c r="AA6" s="43"/>
+      <c r="AB6" s="43"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="43"/>
+      <c r="AE6" s="43"/>
+      <c r="AF6" s="43"/>
+      <c r="AG6" s="43"/>
+      <c r="AH6" s="43"/>
+      <c r="AI6" s="43"/>
+      <c r="AJ6" s="43"/>
+      <c r="AK6" s="43"/>
+      <c r="AL6" s="43"/>
+      <c r="AM6" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN6" s="38"/>
+      <c r="AO6" s="38"/>
+      <c r="AP6" s="38"/>
+      <c r="AQ6" s="38"/>
+      <c r="AR6" s="38"/>
+      <c r="AS6" s="38"/>
+      <c r="AT6" s="38"/>
+      <c r="AU6" s="38"/>
+      <c r="AV6" s="38"/>
+      <c r="AW6" s="38"/>
+      <c r="AX6" s="38"/>
+      <c r="AY6" s="38"/>
+      <c r="AZ6" s="38"/>
+      <c r="BA6" s="38"/>
+      <c r="BB6" s="38"/>
+      <c r="BC6" s="38"/>
+      <c r="BD6" s="38"/>
+      <c r="BE6" s="38"/>
+      <c r="BF6" s="38"/>
+      <c r="BG6" s="38"/>
+      <c r="BH6" s="38"/>
+      <c r="BI6" s="38"/>
+      <c r="BJ6" s="38"/>
+      <c r="BK6" s="38"/>
+      <c r="BL6" s="38"/>
+      <c r="BM6" s="38"/>
+      <c r="BN6" s="38"/>
+      <c r="BO6" s="38"/>
+      <c r="BP6" s="38"/>
+      <c r="BQ6" s="38"/>
+      <c r="BR6" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="BS6" s="36"/>
+      <c r="BT6" s="36"/>
+      <c r="BU6" s="36"/>
+      <c r="BV6" s="36"/>
+      <c r="BW6" s="36"/>
+      <c r="BX6" s="36"/>
+      <c r="BY6" s="36"/>
+      <c r="BZ6" s="36"/>
+      <c r="CA6" s="36"/>
+      <c r="CB6" s="36"/>
+      <c r="CC6" s="36"/>
+      <c r="CD6" s="36"/>
+      <c r="CE6" s="36"/>
+      <c r="CF6" s="36"/>
+      <c r="CG6" s="36"/>
+      <c r="CH6" s="36"/>
+      <c r="CI6" s="36"/>
+      <c r="CJ6" s="36"/>
+      <c r="CK6" s="36"/>
+      <c r="CL6" s="36"/>
+      <c r="CM6" s="36"/>
+      <c r="CN6" s="36"/>
+      <c r="CO6" s="36"/>
+      <c r="CP6" s="36"/>
+      <c r="CQ6" s="36"/>
+      <c r="CR6" s="36"/>
+      <c r="CS6" s="36"/>
+      <c r="CT6" s="36"/>
+      <c r="CU6" s="36"/>
     </row>
     <row r="7" spans="2:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="33"/>
+        <v>25</v>
+      </c>
+      <c r="H7" s="41"/>
       <c r="I7" s="1">
         <v>1</v>
       </c>
@@ -1610,6 +2140,96 @@
       </c>
       <c r="BQ7" s="24">
         <v>31</v>
+      </c>
+      <c r="BR7" s="24">
+        <v>1</v>
+      </c>
+      <c r="BS7" s="24">
+        <v>2</v>
+      </c>
+      <c r="BT7" s="24">
+        <v>3</v>
+      </c>
+      <c r="BU7" s="24">
+        <v>4</v>
+      </c>
+      <c r="BV7" s="24">
+        <v>5</v>
+      </c>
+      <c r="BW7" s="24">
+        <v>6</v>
+      </c>
+      <c r="BX7" s="24">
+        <v>7</v>
+      </c>
+      <c r="BY7" s="24">
+        <v>8</v>
+      </c>
+      <c r="BZ7" s="24">
+        <v>9</v>
+      </c>
+      <c r="CA7" s="24">
+        <v>10</v>
+      </c>
+      <c r="CB7" s="24">
+        <v>11</v>
+      </c>
+      <c r="CC7" s="24">
+        <v>12</v>
+      </c>
+      <c r="CD7" s="24">
+        <v>13</v>
+      </c>
+      <c r="CE7" s="24">
+        <v>14</v>
+      </c>
+      <c r="CF7" s="24">
+        <v>15</v>
+      </c>
+      <c r="CG7" s="24">
+        <v>16</v>
+      </c>
+      <c r="CH7" s="24">
+        <v>17</v>
+      </c>
+      <c r="CI7" s="24">
+        <v>18</v>
+      </c>
+      <c r="CJ7" s="24">
+        <v>19</v>
+      </c>
+      <c r="CK7" s="24">
+        <v>20</v>
+      </c>
+      <c r="CL7" s="24">
+        <v>21</v>
+      </c>
+      <c r="CM7" s="24">
+        <v>22</v>
+      </c>
+      <c r="CN7" s="24">
+        <v>23</v>
+      </c>
+      <c r="CO7" s="24">
+        <v>24</v>
+      </c>
+      <c r="CP7" s="24">
+        <v>25</v>
+      </c>
+      <c r="CQ7" s="24">
+        <v>26</v>
+      </c>
+      <c r="CR7" s="24">
+        <v>27</v>
+      </c>
+      <c r="CS7" s="24">
+        <v>28</v>
+      </c>
+      <c r="CT7" s="24">
+        <v>29</v>
+      </c>
+      <c r="CU7" s="24">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1619,7 +2239,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="34"/>
+      <c r="H8" s="42"/>
       <c r="I8" s="3">
         <v>1</v>
       </c>
@@ -1885,21 +2505,25 @@
         <v>88</v>
       </c>
       <c r="CS8" s="3">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="CT8" s="3">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="CU8" s="3">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="2:99" s="22" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19">
+        <v>88</v>
+      </c>
       <c r="E9" s="19">
         <v>3</v>
       </c>
@@ -1913,20 +2537,20 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
+      <c r="X9" s="37"/>
       <c r="Y9" s="21"/>
       <c r="Z9" s="21"/>
       <c r="AA9" s="21"/>
@@ -1934,7 +2558,7 @@
     </row>
     <row r="10" spans="2:99" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -1951,7 +2575,7 @@
     </row>
     <row r="11" spans="2:99" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1967,7 +2591,7 @@
     </row>
     <row r="12" spans="2:99" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -1983,7 +2607,7 @@
     </row>
     <row r="13" spans="2:99" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1999,7 +2623,7 @@
     </row>
     <row r="14" spans="2:99" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -2015,10 +2639,14 @@
     </row>
     <row r="15" spans="2:99" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="19">
+        <v>1</v>
+      </c>
+      <c r="D15" s="19">
+        <v>88</v>
+      </c>
       <c r="E15" s="19">
         <v>18</v>
       </c>
@@ -2026,8 +2654,8 @@
         <v>33</v>
       </c>
       <c r="G15" s="27">
-        <f>(G16+G17+G18+G19)/4</f>
-        <v>0.89999999999999991</v>
+        <f>(G16+G17+G18+G19+G20)/5</f>
+        <v>0.86</v>
       </c>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
@@ -2053,7 +2681,7 @@
     </row>
     <row r="16" spans="2:99" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -2069,7 +2697,7 @@
     </row>
     <row r="17" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -2085,7 +2713,7 @@
     </row>
     <row r="18" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -2101,7 +2729,7 @@
     </row>
     <row r="19" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -2115,71 +2743,75 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="20" spans="2:28" s="22" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19">
-        <v>51</v>
-      </c>
-      <c r="F20" s="19">
+    <row r="20" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="14">
+        <v>42</v>
+      </c>
+      <c r="F20" s="16">
+        <v>6</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" s="22" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="19">
         <v>1</v>
       </c>
-      <c r="G20" s="20">
-        <f>(G21+G22+G23+G24)/4</f>
+      <c r="D21" s="19">
+        <v>88</v>
+      </c>
+      <c r="E21" s="19">
+        <v>65</v>
+      </c>
+      <c r="F21" s="19">
+        <v>26</v>
+      </c>
+      <c r="G21" s="20">
+        <f>(G22+G23+G25+G26)/4</f>
         <v>0</v>
       </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
-    </row>
-    <row r="21" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14">
-        <v>0</v>
-      </c>
-      <c r="F21" s="14">
-        <v>0</v>
-      </c>
-      <c r="G21" s="15">
-        <v>0</v>
-      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="21"/>
+      <c r="Z21" s="21"/>
+      <c r="AA21" s="21"/>
+      <c r="AB21" s="21"/>
     </row>
     <row r="22" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F22" s="14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G22" s="15">
         <v>0</v>
@@ -2187,15 +2819,15 @@
     </row>
     <row r="23" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F23" s="14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G23" s="15">
         <v>0</v>
@@ -2203,102 +2835,92 @@
     </row>
     <row r="24" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F24" s="14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G24" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="18"/>
+      <c r="B25" s="18" t="s">
+        <v>22</v>
+      </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="15"/>
+      <c r="E25" s="14">
+        <v>70</v>
+      </c>
+      <c r="F25" s="14">
+        <v>15</v>
+      </c>
+      <c r="G25" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="18"/>
+      <c r="B26" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
+      <c r="E26" s="14">
+        <v>85</v>
+      </c>
+      <c r="F26" s="14">
+        <v>5</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="18"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="18"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="18"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
-    </row>
-    <row r="31" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="18"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="18"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="15"/>
-    </row>
-    <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="18"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="18"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15"/>
+    <row r="27" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32">
+        <v>85</v>
+      </c>
+      <c r="F27" s="31">
+        <v>5</v>
+      </c>
+      <c r="G27" s="33">
+        <v>0</v>
+      </c>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
+      <c r="P27" s="34"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="34"/>
+      <c r="T27" s="34"/>
+      <c r="U27" s="34"/>
+      <c r="V27" s="34"/>
+      <c r="W27" s="34"/>
+      <c r="X27" s="34"/>
+      <c r="Y27" s="34"/>
+      <c r="Z27" s="34"/>
+      <c r="AA27" s="34"/>
+      <c r="AB27" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="BR6:CU6"/>
     <mergeCell ref="R9:X9"/>
     <mergeCell ref="AM6:BQ6"/>
     <mergeCell ref="I3:M3"/>
@@ -2306,75 +2928,174 @@
     <mergeCell ref="H2:H8"/>
     <mergeCell ref="I6:AL6"/>
   </mergeCells>
-  <conditionalFormatting sqref="I10:BP34 I9:R9 Y9:BP9">
-    <cfRule type="expression" dxfId="18" priority="11">
+  <conditionalFormatting sqref="I10:BP18 I9:R9 Y9:BP9 I21:CU23 I19:CU19 I25:CU26">
+    <cfRule type="expression" dxfId="49" priority="45">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="13">
+    <cfRule type="expression" dxfId="48" priority="47">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="47" priority="48">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="46" priority="49">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="45" priority="50">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="17">
+    <cfRule type="expression" dxfId="44" priority="51">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="21">
+    <cfRule type="expression" dxfId="43" priority="55">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="22">
+    <cfRule type="expression" dxfId="42" priority="56">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:BP35">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>TRUE</formula>
+  <conditionalFormatting sqref="I8:CR8">
+    <cfRule type="expression" dxfId="41" priority="52">
+      <formula>I$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:CU8">
-    <cfRule type="expression" dxfId="9" priority="18">
+  <conditionalFormatting sqref="BQ9:CR18">
+    <cfRule type="expression" dxfId="40" priority="35">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="37">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="38">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="39">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="40">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="41">
+      <formula>BQ$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="43">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="44">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CS8:CU8">
+    <cfRule type="expression" dxfId="32" priority="34">
+      <formula>CS$8=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CS9:CU18">
+    <cfRule type="expression" dxfId="31" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="27">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="28">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="29">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="30">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="31">
+      <formula>CS$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="32">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="33">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20:CU20">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>I$8=period_selected</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ9:CT34">
-    <cfRule type="expression" dxfId="8" priority="1">
+  <conditionalFormatting sqref="I27:CU27">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="14" priority="10">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>BQ$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>I$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="10">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ35:CT35">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>TRUE</formula>
+  <conditionalFormatting sqref="I24:CU24">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>I$8=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="42" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="32" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">

</xml_diff>